<commit_message>
failed to add filedialog.askopenfilename() to option 1
</commit_message>
<xml_diff>
--- a/Exportados/Domingo_EntradasSalidas.xlsx
+++ b/Exportados/Domingo_EntradasSalidas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
+          <t>MORENO CANCHANYA, ROSMERY</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
+          <t>MORENO CANCHANYA, ROSMERY</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,7 +500,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MEZA PEREZ, JUAN CRISTOFER</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -515,7 +515,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MEZA PEREZ, JUAN CRISTOFER</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -532,118 +532,118 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ZAVALA SOSA, NICOLE</t>
+          <t>SAAVEDRA ALVAN, ANA MARIA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
+          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>07:30</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
+          <t>MEZA MELO, NORMA FERNANDA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
+          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>08:30</t>
+          <t>07:30</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
+          <t>TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>17:15</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>AYALA MORA, CECILIA ROSARIO</t>
+          <t>SAAVEDRA ALVAN, ANA MARIA</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12:30</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>08:45</t>
+          <t>07:00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
+          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>08:30</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -660,86 +660,86 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AYALA MORA, CECILIA ROSARIO</t>
+          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>08:45</t>
+          <t>07:30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>12:30</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
+          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>09:30</t>
+          <t>09:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>07:30</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
+          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>09:45</t>
+          <t>09:30</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HUAMANI TORRES, LUIS RODRIGO</t>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>09:15</t>
+          <t>08:15</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Del Aguila Murayari, Darla</t>
+          <t>YOVERA ROBLES, VICTOR EDUARDO</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -756,22 +756,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
+          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>09:30</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -788,54 +788,54 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
+          <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>09:45</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MORENO CANCHANYA, ROSMERY</t>
+          <t>MEZA PEREZ, JUAN CRISTOFER</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10:15</t>
+          <t>10:30</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>ZAVALA SOSA, NICOLE</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
+          <t>VEGA CARDENAS, ANGELICA LOURDES</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -852,22 +852,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Del Aguila Murayari, Darla</t>
+          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>HUAYANAY VELASCO, ATHINA</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -884,22 +884,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MORENO CANCHANYA, ROSMERY</t>
+          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10:15</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA</t>
+          <t>VEGA RIVAS, ANDREA FERNANDA</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -916,54 +916,54 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>14:15</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
-        </is>
-      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>10:45</t>
+          <t>11:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
+          <t>YOVERA ROBLES, VICTOR EDUARDO</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>14:15</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
+          <t>Del Aguila Murayari, Darla</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -980,22 +980,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
+          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10:45</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
+          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1012,608 +1012,608 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA</t>
+          <t>MEZA PEREZ, JUAN CRISTOFER</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>10:45</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>15:15</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:15</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
+          <t>HUAYANAY VELASCO, ATHINA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
+          <t>VEGA CARDENAS, ANGELICA LOURDES</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
+          <t>VEGA RIVAS, ANDREA FERNANDA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:45</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>AYALA MORA, CECILIA ROSARIO</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>15:15</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ZAVALA SOSA, NICOLE</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:15</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SAAVEDRA ALVAN, ANA MARIA</t>
+          <t>Del Aguila Murayari, Darla</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>20:15</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>17:15</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>12:00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>MEZA MELO, NORMA FERNANDA</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>11:45</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>20:30</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
-        </is>
-      </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>07:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>19:15</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
           <t>12:00</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>15:45</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>HUAMANI TORRES, LUIS RODRIGO</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>09:15</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>AYALA MORA, CECILIA ROSARIO</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>AYALA TAPIA, DARCIE SOL</t>
+          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>11:30</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>CORDOVA MONTALVO, MELANY KARINA</t>
+          <t>TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>07:15</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
+          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>21:15</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>07:15</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>MEDINA MARCELO, NAOMI ARIADNA</t>
+          <t>ZAVALA SOSA, NICOLE</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>09:30</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>SAAVEDRA ALVAN, ANA MARIA</t>
+          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>20:15</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>12:45</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
+          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>20:15</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>08:15</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ZEVALLOS ZANCA, VERONICA LUZ</t>
+          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>22:45</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>CAPCHA YARANGO, DAVID</t>
+          <t>HUAMANI TORRES, LUIS RODRIGO</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>13:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>22:45</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>MEZA MELO, NORMA FERNANDA</t>
+          <t>CORDOVA MONTALVO, MELANY KARINA</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>14:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TITO LAURA, NANCY FIORELLA</t>
+          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>12:45</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
           <t>14:00</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>23:00</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>17:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
+          <t>HUAMANI TORRES, LUIS RODRIGO</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>MEDINA MARCELO, NAOMI ARIADNA</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
           <t>14:00</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>17:45</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>VARGAS CASTRO, LOANA VICTORIA</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>17:00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>AYALA TAPIA, DARCIE SOL</t>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
+          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>21:15</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>10:15</t>
         </is>
       </c>
     </row>
@@ -1625,66 +1625,66 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
+          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>21:15</t>
+          <t>19:15</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>11:00</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+          <t>CORDOVA MONTALVO, MELANY KARINA</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
           <t>15:45</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>19:30</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>INGA DELGADO, CARLOS DANIEL</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>21:30</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>17:45</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CORDOVA MONTALVO, MELANY KARINA</t>
+          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1694,98 +1694,98 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
+          <t>FLORES PAREDES, LOURDES</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>19:45</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>16:00</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
+          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>20:15</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
+          <t>VILCHEZ CUBA, JACK ANTHONY</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CAPCHA YARANGO, DAVID</t>
+          <t>FLORES PAREDES, LOURDES</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>19:45</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
+          <t>VARGAS CASTRO, LOANA VICTORIA</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>VARGAS CASTRO, LOANA VICTORIA</t>
+          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1800,93 +1800,93 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
+          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>20:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
+          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
+          <t>YACILA GRANDEZ, RODRIGO ANDRE</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>21:15</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
+          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>INGA DELGADO, CARLOS DANIEL</t>
+          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1896,236 +1896,524 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
+          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
+          <t>BRENIS LÁRTIGA, SEBASTIÁN</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
+          <t>BRENIS LÁRTIGA, SEBASTIÁN</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
+          <t>AYALA TAPIA, DARCIE SOL</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
+          <t>VILCHEZ CUBA, JACK ANTHONY</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
+          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>18:15</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>PARICELA TINEO, JAIME DANIEL</t>
+          <t>AYALA TAPIA, DARCIE SOL</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>ZEVALLOS ZANCA, VERONICA LUZ</t>
+          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>22:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>15:45</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>YACILA GRANDEZ, RODRIGO ANDRE</t>
+          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
+          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>22:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>10:00</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
+          <t>VARGAS CASTRO, LOANA VICTORIA</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>18:15</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO</t>
+          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>22:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>PARICELA TINEO, JAIME DANIEL</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>CAPCHA YARANGO, DAVID</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>22:45</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>TITO LAURA, NANCY FIORELLA</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>23:00</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>14:00</t>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>INGA DELGADO, CARLOS DANIEL</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>INGA DELGADO, CARLOS DANIEL</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CAPCHA YARANGO, DAVID</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>YANAC DAVILA, GERALD RONNY</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>YANAC DAVILA, GERALD RONNY</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>17:15</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added option 11 and fixed error of don't showing option 10 EAN
</commit_message>
<xml_diff>
--- a/Exportados/Domingo_EntradasSalidas.xlsx
+++ b/Exportados/Domingo_EntradasSalidas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MORENO CANCHANYA, ROSMERY</t>
+          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MORENO CANCHANYA, ROSMERY</t>
+          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,7 +500,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>MEZA PEREZ, JUAN CRISTOFER</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -515,7 +515,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>MEZA PEREZ, JUAN CRISTOFER</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -532,118 +532,118 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SAAVEDRA ALVAN, ANA MARIA</t>
+          <t>ZAVALA SOSA, NICOLE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>16:45</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>12:00</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>11:15</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>07:30</t>
+          <t>08:15</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MEZA MELO, NORMA FERNANDA</t>
+          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>08:15</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:15</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>07:30</t>
+          <t>08:30</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TITO LAURA, NANCY FIORELLA</t>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>08:15</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SAAVEDRA ALVAN, ANA MARIA</t>
+          <t>AYALA MORA, CECILIA ROSARIO</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>12:30</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>08:45</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>12:15</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -660,86 +660,86 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
+          <t>AYALA MORA, CECILIA ROSARIO</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>07:30</t>
+          <t>08:45</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:30</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
+          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>09:30</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>07:30</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
+          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>09:30</t>
+          <t>09:45</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
+          <t>HUAMANI TORRES, LUIS RODRIGO</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>09:15</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17:15</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>YOVERA ROBLES, VICTOR EDUARDO</t>
+          <t>Del Aguila Murayari, Darla</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -756,22 +756,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
+          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -788,54 +788,54 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
+          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>09:45</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MEZA PEREZ, JUAN CRISTOFER</t>
+          <t>MORENO CANCHANYA, ROSMERY</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>14:15</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>10:15</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ZAVALA SOSA, NICOLE</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>09:30</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>VEGA CARDENAS, ANGELICA LOURDES</t>
+          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -852,22 +852,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
+          <t>Del Aguila Murayari, Darla</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>09:30</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -884,22 +884,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
+          <t>MORENO CANCHANYA, ROSMERY</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>VEGA RIVAS, ANDREA FERNANDA</t>
+          <t>HUAYANAY VELASCO, ATHINA</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -916,54 +916,54 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:45</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>YOVERA ROBLES, VICTOR EDUARDO</t>
+          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Del Aguila Murayari, Darla</t>
+          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -980,22 +980,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
+          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10:15</t>
+          <t>10:45</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
+          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1012,608 +1012,608 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MEZA PEREZ, JUAN CRISTOFER</t>
+          <t>HUAYANAY VELASCO, ATHINA</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>10:45</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14:15</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>11:30</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA</t>
+          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14:15</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:00</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>VEGA CARDENAS, ANGELICA LOURDES</t>
+          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14:15</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>VEGA RIVAS, ANDREA FERNANDA</t>
+          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>10:45</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>AYALA MORA, CECILIA ROSARIO</t>
+          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:00</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>ZAVALA SOSA, NICOLE</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>08:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Del Aguila Murayari, Darla</t>
+          <t>SAAVEDRA ALVAN, ANA MARIA</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>20:15</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>08:15</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>MEZA MELO, NORMA FERNANDA</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>MEZA MELO, NORMA FERNANDA</t>
+          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
+          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>19:15</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
+          <t>HUAMANI TORRES, LUIS RODRIGO</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:15</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AYALA MORA, CECILIA ROSARIO</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>AYALA TAPIA, DARCIE SOL</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
           <t>15:00</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>11:30</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>TITO LAURA, NANCY FIORELLA</t>
+          <t>CORDOVA MONTALVO, MELANY KARINA</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>15:45</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
+          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:15</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>21:15</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>15:45</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
+          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ZAVALA SOSA, NICOLE</t>
+          <t>MEDINA MARCELO, NAOMI ARIADNA</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>09:30</t>
+          <t>15:45</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
+          <t>SAAVEDRA ALVAN, ANA MARIA</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>20:15</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>11:30</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
+          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
+          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>17:15</t>
+          <t>20:15</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>16:30</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
+          <t>ZEVALLOS ZANCA, VERONICA LUZ</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>22:45</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>HUAMANI TORRES, LUIS RODRIGO</t>
+          <t>CAPCHA YARANGO, DAVID</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:45</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>22:45</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>CORDOVA MONTALVO, MELANY KARINA</t>
+          <t>MEZA MELO, NORMA FERNANDA</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:45</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
+          <t>TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>23:00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>HUAMANI TORRES, LUIS RODRIGO</t>
+          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>MEDINA MARCELO, NAOMI ARIADNA</t>
+          <t>VARGAS CASTRO, LOANA VICTORIA</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+          <t>AYALA TAPIA, DARCIE SOL</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
+          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>21:15</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>10:15</t>
+          <t>17:30</t>
         </is>
       </c>
     </row>
@@ -1625,66 +1625,66 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
+          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>19:15</t>
+          <t>21:15</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:15</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CORDOVA MONTALVO, MELANY KARINA</t>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>INGA DELGADO, CARLOS DANIEL</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
           <t>17:45</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>19:30</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>15:45</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
+          <t>CORDOVA MONTALVO, MELANY KARINA</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1694,98 +1694,98 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>FLORES PAREDES, LOURDES</t>
+          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>19:45</t>
+          <t>21:30</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:45</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
+          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>20:15</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>VILCHEZ CUBA, JACK ANTHONY</t>
+          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:00</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>FLORES PAREDES, LOURDES</t>
+          <t>CAPCHA YARANGO, DAVID</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>19:45</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>VARGAS CASTRO, LOANA VICTORIA</t>
+          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>13:15</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
+          <t>VARGAS CASTRO, LOANA VICTORIA</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1800,93 +1800,93 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:00</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
+          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
+          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>13:00</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>YACILA GRANDEZ, RODRIGO ANDRE</t>
+          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:15</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
+          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:00</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
+          <t>INGA DELGADO, CARLOS DANIEL</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:30</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1896,524 +1896,236 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:00</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:30</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>BRENIS LÁRTIGA, SEBASTIÁN</t>
+          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>13:00</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>BRENIS LÁRTIGA, SEBASTIÁN</t>
+          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>AYALA TAPIA, DARCIE SOL</t>
+          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>11:00</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>VILCHEZ CUBA, JACK ANTHONY</t>
+          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
+          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:15</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>AYALA TAPIA, DARCIE SOL</t>
+          <t>PARICELA TINEO, JAIME DANIEL</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
+          <t>ZEVALLOS ZANCA, VERONICA LUZ</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>22:45</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>13:45</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
+          <t>YACILA GRANDEZ, RODRIGO ANDRE</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
+          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>22:45</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:45</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>VARGAS CASTRO, LOANA VICTORIA</t>
+          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:15</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>22:45</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>19:00</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>PARICELA TINEO, JAIME DANIEL</t>
+          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>22:45</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>CAPCHA YARANGO, DAVID</t>
+          <t>TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>20:45</t>
+          <t>23:00</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>INGA DELGADO, CARLOS DANIEL</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>INGA DELGADO, CARLOS DANIEL</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>CAPCHA YARANGO, DAVID</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>YANAC DAVILA, GERALD RONNY</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>YANAC DAVILA, GERALD RONNY</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>17:15</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>21:00</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>21:00</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>17:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>17:15</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>21:00</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>21:00</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>17:15</t>
+          <t>14:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added case with comillas in pdf_path in option 1
</commit_message>
<xml_diff>
--- a/Exportados/Domingo_EntradasSalidas.xlsx
+++ b/Exportados/Domingo_EntradasSalidas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
+          <t>MORENO CANCHANYA, ROSMERY</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
+          <t>MORENO CANCHANYA, ROSMERY</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,7 +500,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MEZA PEREZ, JUAN CRISTOFER</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -515,7 +515,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MEZA PEREZ, JUAN CRISTOFER</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -532,118 +532,118 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ZAVALA SOSA, NICOLE</t>
+          <t>SAAVEDRA ALVAN, ANA MARIA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
+          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>07:30</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
+          <t>MEZA MELO, NORMA FERNANDA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
+          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>08:30</t>
+          <t>07:30</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
+          <t>TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>17:15</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>AYALA MORA, CECILIA ROSARIO</t>
+          <t>SAAVEDRA ALVAN, ANA MARIA</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12:30</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>08:45</t>
+          <t>07:00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
+          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>08:30</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -660,86 +660,86 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AYALA MORA, CECILIA ROSARIO</t>
+          <t>AGUILAR SCHLAEFLI, STEPHANIE XIMENA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>08:45</t>
+          <t>07:30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>12:30</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
+          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>09:30</t>
+          <t>09:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>07:30</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
+          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>09:45</t>
+          <t>09:30</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HUAMANI TORRES, LUIS RODRIGO</t>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>09:15</t>
+          <t>08:15</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Del Aguila Murayari, Darla</t>
+          <t>YOVERA ROBLES, VICTOR EDUARDO</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -756,22 +756,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
+          <t>POBLETE SAIRE, FIORELLA ESTHER</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>09:30</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -788,54 +788,54 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
+          <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>09:45</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MORENO CANCHANYA, ROSMERY</t>
+          <t>MEZA PEREZ, JUAN CRISTOFER</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10:15</t>
+          <t>10:30</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>ZAVALA SOSA, NICOLE</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
+          <t>VEGA CARDENAS, ANGELICA LOURDES</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -852,22 +852,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Del Aguila Murayari, Darla</t>
+          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>HUAYANAY VELASCO, ATHINA</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -884,22 +884,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MORENO CANCHANYA, ROSMERY</t>
+          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10:15</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA</t>
+          <t>VEGA RIVAS, ANDREA FERNANDA</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -916,54 +916,54 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>14:15</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
-        </is>
-      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>10:45</t>
+          <t>11:00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL</t>
+          <t>YOVERA ROBLES, VICTOR EDUARDO</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>14:15</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
+          <t>Del Aguila Murayari, Darla</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -980,22 +980,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MONTEZUMA DEJO, EVELYN BRUNELLA</t>
+          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10:45</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
+          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1012,608 +1012,608 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA</t>
+          <t>MEZA PEREZ, JUAN CRISTOFER</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>10:45</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>15:15</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:15</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
+          <t>HUAYANAY VELASCO, ATHINA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGÓN, JUAN ALFONSO</t>
+          <t>VEGA CARDENAS, ANGELICA LOURDES</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
+          <t>VEGA RIVAS, ANDREA FERNANDA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:45</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>AYALA MORA, CECILIA ROSARIO</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>15:15</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ZAVALA SOSA, NICOLE</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:15</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SAAVEDRA ALVAN, ANA MARIA</t>
+          <t>Del Aguila Murayari, Darla</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>20:15</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>17:15</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>12:00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>MEZA MELO, NORMA FERNANDA</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>11:45</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>20:30</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
-        </is>
-      </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>07:00</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>19:15</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
           <t>12:00</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>15:45</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>HUAMANI TORRES, LUIS RODRIGO</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>09:15</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>AYALA MORA, CECILIA ROSARIO</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>AYALA TAPIA, DARCIE SOL</t>
+          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>11:30</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SUAREZ JARA, YENNIFER YUSSARA</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>CORDOVA MONTALVO, MELANY KARINA</t>
+          <t>TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>07:15</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
+          <t>GOMEZ ALBINO, IDALIA GIMENA</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>21:15</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>07:15</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>MEDINA MARCELO, NAOMI ARIADNA</t>
+          <t>ZAVALA SOSA, NICOLE</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>09:30</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>SAAVEDRA ALVAN, ANA MARIA</t>
+          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>20:15</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>12:45</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
+          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>20:15</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>08:15</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ZEVALLOS ZANCA, VERONICA LUZ</t>
+          <t>CHIARA LIMA, AUGUSTO SEBASTIAN</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>22:45</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>CAPCHA YARANGO, DAVID</t>
+          <t>HUAMANI TORRES, LUIS RODRIGO</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>13:00</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>22:45</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>MEZA MELO, NORMA FERNANDA</t>
+          <t>CORDOVA MONTALVO, MELANY KARINA</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>14:00</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TITO LAURA, NANCY FIORELLA</t>
+          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>12:45</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
           <t>14:00</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>23:00</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>17:00</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
+          <t>HUAMANI TORRES, LUIS RODRIGO</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>MEDINA MARCELO, NAOMI ARIADNA</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
           <t>14:00</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>17:45</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>VARGAS CASTRO, LOANA VICTORIA</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>20:45</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>17:00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>AYALA TAPIA, DARCIE SOL</t>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
+          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>21:15</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>10:15</t>
         </is>
       </c>
     </row>
@@ -1625,66 +1625,66 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>CHAVEZ ONOFRE, CAMILA GERALDINE</t>
+          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>21:15</t>
+          <t>19:15</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>11:00</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+          <t>CORDOVA MONTALVO, MELANY KARINA</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
           <t>15:45</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>19:30</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>INGA DELGADO, CARLOS DANIEL</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>21:30</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>17:45</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CORDOVA MONTALVO, MELANY KARINA</t>
+          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1694,98 +1694,98 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
+          <t>FLORES PAREDES, LOURDES</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>19:45</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>16:00</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
+          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>20:15</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
+          <t>VILCHEZ CUBA, JACK ANTHONY</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CAPCHA YARANGO, DAVID</t>
+          <t>FLORES PAREDES, LOURDES</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>19:45</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
+          <t>VARGAS CASTRO, LOANA VICTORIA</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>VARGAS CASTRO, LOANA VICTORIA</t>
+          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1800,93 +1800,93 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
+          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>20:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
+          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MARTICORENA LOPEZ, DAVID CARLOS</t>
+          <t>YACILA GRANDEZ, RODRIGO ANDRE</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>21:15</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
+          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>INGA DELGADO, CARLOS DANIEL</t>
+          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1896,236 +1896,524 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
+          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>SOTELO GONZALES, CAMILA SOFÍA</t>
+          <t>BRENIS LÁRTIGA, SEBASTIÁN</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>HUAYNATES ALTAMIRANO, JIM HANS</t>
+          <t>BRENIS LÁRTIGA, SEBASTIÁN</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
+          <t>AYALA TAPIA, DARCIE SOL</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
+          <t>VILCHEZ CUBA, JACK ANTHONY</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
+          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>18:15</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>PARICELA TINEO, JAIME DANIEL</t>
+          <t>AYALA TAPIA, DARCIE SOL</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>ZEVALLOS ZANCA, VERONICA LUZ</t>
+          <t>HINOSTROZA MARIN, CAMILA MARIA</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>22:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>15:45</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>YACILA GRANDEZ, RODRIGO ANDRE</t>
+          <t>ARIAS MACHACUAY, SADELITH SORAGGI</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
+          <t>BRICEÑO LUNA, JESSICA ARACELI</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>22:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>10:00</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>SALAS VILLANUEVA, JAMILA DASHA</t>
+          <t>VARGAS CASTRO, LOANA VICTORIA</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>18:15</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>22:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO</t>
+          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>22:45</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>16:15</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>PARICELA TINEO, JAIME DANIEL</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>CAPCHA YARANGO, DAVID</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>22:45</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>TITO LAURA, NANCY FIORELLA</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>23:00</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>14:00</t>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>INGA DELGADO, CARLOS DANIEL</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>INGA DELGADO, CARLOS DANIEL</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CAPCHA YARANGO, DAVID</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>MENDOZA DIEGO, ZAIDA VANESSA</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>YANAC DAVILA, GERALD RONNY</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>YANAC DAVILA, GERALD RONNY</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>MENDOZA CRUZ, LILIANA LILIANA</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>RIVERA CARREÑO, DIANA DESIRÉE</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>17:15</t>
         </is>
       </c>
     </row>

</xml_diff>